<commit_message>
updated participant log 8/24
</commit_message>
<xml_diff>
--- a/data/01_participant_logs/es_combined_subject_log.xlsx
+++ b/data/01_participant_logs/es_combined_subject_log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Experiments/KM_SPEED_ACC_NOVEL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethswanson/Documents/speed-acc-novel/data/01_participant_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CD671D-087A-4140-B21A-275600036F91}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45403BF3-20C1-3343-A224-0A05C30122B2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25480" windowHeight="14780" xr2:uid="{C7933D04-C61A-4F49-A5A3-D50AD8D5C7BA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25480" windowHeight="14760" xr2:uid="{C7933D04-C61A-4F49-A5A3-D50AD8D5C7BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="256">
   <si>
     <t>subid</t>
   </si>
@@ -736,6 +736,63 @@
   </si>
   <si>
     <t>LK</t>
+  </si>
+  <si>
+    <t>SAN-082018-04</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>A, C?</t>
+  </si>
+  <si>
+    <t>Aunt sat nearby; didn't seem to cause any problems</t>
+  </si>
+  <si>
+    <t>SAN-082018-05</t>
+  </si>
+  <si>
+    <t>I, C?</t>
+  </si>
+  <si>
+    <t>Asked to stop during 3rd word block; lots of trouble with headphones during 2nd block; moved around a lot</t>
+  </si>
+  <si>
+    <t>SAN-082218-01</t>
+  </si>
+  <si>
+    <t>Es</t>
+  </si>
+  <si>
+    <t>SAN-082218-02</t>
+  </si>
+  <si>
+    <t>KD</t>
+  </si>
+  <si>
+    <t>Said words out loud; also, seemed to consistently point/look to wrong object during SA trials</t>
+  </si>
+  <si>
+    <t>SAN-082318-01</t>
+  </si>
+  <si>
+    <t>TJ</t>
+  </si>
+  <si>
+    <t>SAN-082318-02</t>
+  </si>
+  <si>
+    <t>AJ</t>
+  </si>
+  <si>
+    <t>Asked to stop about 1/4 of way through; can't find .idf file for some reason</t>
+  </si>
+  <si>
+    <t>SAN-082418-01</t>
+  </si>
+  <si>
+    <t>FS</t>
   </si>
 </sst>
 </file>
@@ -1142,10 +1199,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3EC3C8B-E78F-3A47-8874-F07602A94D1E}">
-  <dimension ref="A1:Q89"/>
+  <dimension ref="A1:Q96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="L59" sqref="L59"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3771,7 +3828,6 @@
         <v>42218</v>
       </c>
       <c r="F55" s="3">
-        <f t="shared" ref="F55:F57" si="4">ROUND(YEARFRAC(E55,D55), 3)</f>
         <v>3.0419999999999998</v>
       </c>
       <c r="G55" s="3" t="s">
@@ -3820,7 +3876,6 @@
         <v>41660</v>
       </c>
       <c r="F56" s="3">
-        <f t="shared" si="4"/>
         <v>4.5810000000000004</v>
       </c>
       <c r="G56" s="3" t="s">
@@ -3869,7 +3924,6 @@
         <v>41787</v>
       </c>
       <c r="F57" s="3">
-        <f t="shared" si="4"/>
         <v>4.2279999999999998</v>
       </c>
       <c r="G57" s="3" t="s">
@@ -3918,7 +3972,6 @@
         <v>41606</v>
       </c>
       <c r="F58" s="3">
-        <f t="shared" ref="F58" si="5">ROUND(YEARFRAC(E58,D58), 3)</f>
         <v>4.7279999999999998</v>
       </c>
       <c r="G58" s="3" t="s">
@@ -3952,178 +4005,181 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>158</v>
+        <v>237</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>159</v>
+        <v>238</v>
       </c>
       <c r="D59" s="4">
-        <v>43301</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F59" s="4" t="s">
-        <v>21</v>
+        <v>43332</v>
+      </c>
+      <c r="E59" s="4">
+        <v>42018</v>
+      </c>
+      <c r="F59" s="3">
+        <v>3.6</v>
       </c>
       <c r="G59" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>81</v>
+        <v>239</v>
       </c>
       <c r="I59" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J59" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K59" s="10" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="L59" s="3" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="M59" s="3" t="s">
-        <v>160</v>
+        <v>21</v>
       </c>
       <c r="N59" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O59" s="3" t="s">
-        <v>161</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="P59" s="3"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>162</v>
+        <v>241</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>163</v>
+        <v>238</v>
       </c>
       <c r="D60" s="4">
-        <v>43301</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>21</v>
+        <v>43332</v>
+      </c>
+      <c r="E60" s="4">
+        <v>41844</v>
+      </c>
+      <c r="F60" s="3">
+        <v>4.0720000000000001</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>81</v>
+        <v>242</v>
       </c>
       <c r="I60" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J60" s="3">
+        <v>4</v>
+      </c>
+      <c r="K60" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="L60" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M60" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N60" s="3">
         <v>2</v>
       </c>
-      <c r="K60" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="L60" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M60" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="N60" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="O60" s="3" t="s">
-        <v>165</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="P60" s="3"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>166</v>
+        <v>244</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
       <c r="D61" s="4">
-        <v>43301</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F61" s="4" t="s">
-        <v>21</v>
+        <v>43334</v>
+      </c>
+      <c r="E61" s="4">
+        <v>42237</v>
+      </c>
+      <c r="F61" s="3">
+        <v>3.0030000000000001</v>
       </c>
       <c r="G61" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>81</v>
+        <v>239</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>17</v>
+        <v>245</v>
       </c>
       <c r="J61" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K61" s="10" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="L61" s="3" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="M61" s="3" t="s">
-        <v>164</v>
+        <v>21</v>
       </c>
       <c r="N61" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O61" s="3" t="s">
-        <v>168</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="P61" s="3"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>169</v>
+        <v>246</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>170</v>
+        <v>247</v>
       </c>
       <c r="D62" s="4">
-        <v>43306</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>21</v>
+        <v>43334</v>
+      </c>
+      <c r="E62" s="4">
+        <v>41223</v>
+      </c>
+      <c r="F62" s="3">
+        <v>5.7830000000000004</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>81</v>
+        <v>239</v>
       </c>
       <c r="I62" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J62" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K62" s="10" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="L62" s="3" t="s">
         <v>40</v>
@@ -4135,48 +4191,49 @@
         <v>21</v>
       </c>
       <c r="O62" s="3" t="s">
-        <v>171</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="P62" s="3"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>172</v>
+        <v>249</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>173</v>
+        <v>250</v>
       </c>
       <c r="D63" s="4">
-        <v>43306</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F63" s="4" t="s">
-        <v>21</v>
+        <v>43335</v>
+      </c>
+      <c r="E63" s="4">
+        <v>42229</v>
+      </c>
+      <c r="F63" s="3">
+        <v>3.028</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>26</v>
+        <v>239</v>
       </c>
       <c r="I63" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J63" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K63" s="10" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>174</v>
+        <v>21</v>
       </c>
       <c r="N63" s="3" t="s">
         <v>21</v>
@@ -4184,113 +4241,116 @@
       <c r="O63" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="P63" s="3"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>175</v>
+        <v>251</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>176</v>
+        <v>252</v>
       </c>
       <c r="D64" s="4">
-        <v>43306</v>
-      </c>
-      <c r="E64" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F64" s="4" t="s">
-        <v>21</v>
+        <v>43335</v>
+      </c>
+      <c r="E64" s="4">
+        <v>41248</v>
+      </c>
+      <c r="F64" s="3">
+        <v>5.7169999999999996</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>81</v>
+        <v>239</v>
       </c>
       <c r="I64" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J64" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K64" s="10" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="L64" s="3" t="s">
         <v>19</v>
       </c>
       <c r="M64" s="3" t="s">
-        <v>174</v>
+        <v>21</v>
       </c>
       <c r="N64" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O64" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="P64" s="3"/>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>177</v>
+        <v>254</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>178</v>
+        <v>255</v>
       </c>
       <c r="D65" s="4">
-        <v>43306</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F65" s="4" t="s">
-        <v>21</v>
+        <v>43336</v>
+      </c>
+      <c r="E65" s="4">
+        <v>42126</v>
+      </c>
+      <c r="F65" s="3">
+        <v>3.3109999999999999</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>81</v>
+        <v>220</v>
       </c>
       <c r="I65" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J65" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K65" s="10" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="L65" s="3" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="M65" s="3" t="s">
-        <v>174</v>
+        <v>21</v>
       </c>
       <c r="N65" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O65" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="P65" s="3"/>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="D66" s="4">
-        <v>43308</v>
+        <v>43301</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>21</v>
@@ -4314,30 +4374,30 @@
         <v>18</v>
       </c>
       <c r="L66" s="3" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="M66" s="3" t="s">
-        <v>21</v>
+        <v>160</v>
       </c>
       <c r="N66" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O66" s="3" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="D67" s="4">
-        <v>43308</v>
+        <v>43301</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>21</v>
@@ -4364,27 +4424,27 @@
         <v>19</v>
       </c>
       <c r="M67" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="N67" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O67" s="3" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>84</v>
+        <v>167</v>
       </c>
       <c r="D68" s="4">
-        <v>43308</v>
+        <v>43301</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>21</v>
@@ -4411,27 +4471,27 @@
         <v>19</v>
       </c>
       <c r="M68" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="N68" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O68" s="3" t="s">
-        <v>21</v>
+        <v>168</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="D69" s="4">
-        <v>43313</v>
+        <v>43306</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>21</v>
@@ -4443,16 +4503,16 @@
         <v>15</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="I69" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J69" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K69" s="10" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="L69" s="3" t="s">
         <v>40</v>
@@ -4464,21 +4524,21 @@
         <v>21</v>
       </c>
       <c r="O69" s="3" t="s">
-        <v>21</v>
+        <v>171</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="D70" s="4">
-        <v>43313</v>
+        <v>43306</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>21</v>
@@ -4487,25 +4547,25 @@
         <v>21</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>190</v>
+        <v>26</v>
       </c>
       <c r="I70" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J70" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K70" s="10" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="L70" s="3" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="M70" s="3" t="s">
-        <v>21</v>
+        <v>174</v>
       </c>
       <c r="N70" s="3" t="s">
         <v>21</v>
@@ -4513,20 +4573,19 @@
       <c r="O70" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="P70" s="3"/>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="D71" s="4">
-        <v>43313</v>
+        <v>43306</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>21</v>
@@ -4535,47 +4594,45 @@
         <v>21</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="I71" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J71" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K71" s="10" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="L71" s="3" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="M71" s="3" t="s">
-        <v>21</v>
+        <v>174</v>
       </c>
       <c r="N71" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O71" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="P71" s="3"/>
-      <c r="Q71" s="3"/>
+        <v>21</v>
+      </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="D72" s="4">
-        <v>43313</v>
+        <v>43306</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>21</v>
@@ -4584,7 +4641,7 @@
         <v>21</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>81</v>
@@ -4593,10 +4650,10 @@
         <v>17</v>
       </c>
       <c r="J72" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K72" s="10" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="L72" s="3" t="s">
         <v>19</v>
@@ -4610,21 +4667,19 @@
       <c r="O72" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="P72" s="3"/>
-      <c r="Q72" s="3"/>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>117</v>
+        <v>180</v>
       </c>
       <c r="D73" s="4">
-        <v>43315</v>
+        <v>43308</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>21</v>
@@ -4633,7 +4688,7 @@
         <v>21</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H73" s="3" t="s">
         <v>81</v>
@@ -4642,10 +4697,10 @@
         <v>17</v>
       </c>
       <c r="J73" s="3">
-        <v>4</v>
-      </c>
-      <c r="K73" s="3" t="s">
-        <v>50</v>
+        <v>1</v>
+      </c>
+      <c r="K73" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="L73" s="3" t="s">
         <v>40</v>
@@ -4657,23 +4712,21 @@
         <v>21</v>
       </c>
       <c r="O73" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P73" s="3"/>
-      <c r="Q73" s="3"/>
+        <v>181</v>
+      </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="D74" s="4">
-        <v>43315</v>
+        <v>43308</v>
       </c>
       <c r="E74" s="4" t="s">
         <v>21</v>
@@ -4685,44 +4738,42 @@
         <v>15</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="I74" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J74" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K74" s="10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="L74" s="3" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="M74" s="3" t="s">
-        <v>21</v>
+        <v>174</v>
       </c>
       <c r="N74" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O74" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P74" s="3"/>
-      <c r="Q74" s="3"/>
+        <v>184</v>
+      </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>200</v>
+        <v>84</v>
       </c>
       <c r="D75" s="4">
-        <v>43318</v>
+        <v>43308</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>21</v>
@@ -4734,44 +4785,42 @@
         <v>25</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="I75" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J75" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K75" s="10" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="L75" s="3" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="M75" s="3" t="s">
-        <v>21</v>
+        <v>174</v>
       </c>
       <c r="N75" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O75" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="P75" s="3"/>
-      <c r="Q75" s="3"/>
+        <v>21</v>
+      </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="D76" s="4">
-        <v>43320</v>
+        <v>43313</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>21</v>
@@ -4780,7 +4829,7 @@
         <v>21</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H76" s="3" t="s">
         <v>77</v>
@@ -4789,10 +4838,10 @@
         <v>17</v>
       </c>
       <c r="J76" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K76" s="10" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="L76" s="3" t="s">
         <v>40</v>
@@ -4804,23 +4853,21 @@
         <v>21</v>
       </c>
       <c r="O76" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="P76" s="3"/>
-      <c r="Q76" s="3"/>
+        <v>21</v>
+      </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="D77" s="4">
-        <v>43322</v>
+        <v>43313</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>21</v>
@@ -4829,165 +4876,374 @@
         <v>21</v>
       </c>
       <c r="G77" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H77" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="I77" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J77" s="3">
+        <v>1</v>
+      </c>
+      <c r="K77" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L77" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M77" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N77" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O77" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P77" s="3"/>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D78" s="4">
+        <v>43313</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G78" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H77" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="I77" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J77" s="3">
+      <c r="H78" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I78" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J78" s="3">
         <v>2</v>
       </c>
-      <c r="K77" s="10" t="s">
+      <c r="K78" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="L77" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="M77" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N77" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="O77" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="P77" s="3"/>
-      <c r="Q77" s="3"/>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A78" s="3"/>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="4"/>
-      <c r="E78" s="4"/>
-      <c r="F78" s="4"/>
-      <c r="G78" s="3"/>
-      <c r="H78" s="3"/>
-      <c r="I78" s="3"/>
-      <c r="J78" s="3"/>
-      <c r="K78" s="10"/>
-      <c r="L78" s="3"/>
-      <c r="M78" s="3"/>
-      <c r="N78" s="3"/>
-      <c r="O78" s="3"/>
+      <c r="L78" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M78" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N78" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O78" s="3" t="s">
+        <v>193</v>
+      </c>
       <c r="P78" s="3"/>
       <c r="Q78" s="3"/>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A79" s="3"/>
-      <c r="B79" s="3"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="4"/>
-      <c r="G79" s="3"/>
-      <c r="H79" s="3"/>
-      <c r="I79" s="3"/>
-      <c r="J79" s="3"/>
-      <c r="K79" s="10"/>
-      <c r="L79" s="3"/>
-      <c r="M79" s="3"/>
-      <c r="N79" s="3"/>
-      <c r="O79" s="3"/>
+      <c r="A79" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D79" s="4">
+        <v>43313</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H79" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I79" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J79" s="3">
+        <v>3</v>
+      </c>
+      <c r="K79" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="L79" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M79" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="N79" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O79" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="P79" s="3"/>
       <c r="Q79" s="3"/>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A80" s="3"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="4"/>
-      <c r="E80" s="4"/>
-      <c r="F80" s="4"/>
-      <c r="G80" s="3"/>
-      <c r="H80" s="3"/>
-      <c r="I80" s="3"/>
-      <c r="J80" s="3"/>
-      <c r="K80" s="10"/>
-      <c r="L80" s="3"/>
-      <c r="M80" s="3"/>
-      <c r="N80" s="3"/>
-      <c r="O80" s="3"/>
+      <c r="A80" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D80" s="4">
+        <v>43315</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H80" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I80" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J80" s="3">
+        <v>4</v>
+      </c>
+      <c r="K80" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L80" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M80" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N80" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O80" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="P80" s="3"/>
       <c r="Q80" s="3"/>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A81" s="3"/>
-      <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="4"/>
-      <c r="E81" s="4"/>
-      <c r="F81" s="4"/>
-      <c r="G81" s="3"/>
-      <c r="H81" s="3"/>
-      <c r="I81" s="3"/>
-      <c r="J81" s="3"/>
-      <c r="K81" s="10"/>
-      <c r="L81" s="3"/>
-      <c r="M81" s="3"/>
-      <c r="N81" s="3"/>
-      <c r="O81" s="3"/>
+      <c r="A81" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D81" s="4">
+        <v>43315</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I81" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J81" s="3">
+        <v>3</v>
+      </c>
+      <c r="K81" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="L81" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M81" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N81" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O81" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="P81" s="3"/>
       <c r="Q81" s="3"/>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A82" s="3"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="4"/>
-      <c r="E82" s="4"/>
-      <c r="F82" s="4"/>
-      <c r="G82" s="3"/>
-      <c r="H82" s="3"/>
-      <c r="I82" s="3"/>
-      <c r="J82" s="3"/>
-      <c r="K82" s="10"/>
-      <c r="L82" s="3"/>
-      <c r="M82" s="3"/>
-      <c r="N82" s="3"/>
-      <c r="O82" s="3"/>
+      <c r="A82" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D82" s="4">
+        <v>43318</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I82" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J82" s="3">
+        <v>2</v>
+      </c>
+      <c r="K82" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="L82" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M82" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N82" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O82" s="3" t="s">
+        <v>201</v>
+      </c>
       <c r="P82" s="3"/>
       <c r="Q82" s="3"/>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A83" s="3"/>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="4"/>
-      <c r="E83" s="4"/>
-      <c r="F83" s="4"/>
-      <c r="G83" s="3"/>
-      <c r="H83" s="3"/>
-      <c r="I83" s="3"/>
-      <c r="J83" s="3"/>
-      <c r="K83" s="10"/>
-      <c r="L83" s="3"/>
-      <c r="M83" s="3"/>
-      <c r="N83" s="3"/>
-      <c r="O83" s="3"/>
+      <c r="A83" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D83" s="4">
+        <v>43320</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I83" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J83" s="3">
+        <v>1</v>
+      </c>
+      <c r="K83" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L83" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M83" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N83" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O83" s="3" t="s">
+        <v>204</v>
+      </c>
       <c r="P83" s="3"/>
       <c r="Q83" s="3"/>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A84" s="3"/>
-      <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
-      <c r="D84" s="4"/>
-      <c r="E84" s="4"/>
-      <c r="F84" s="4"/>
-      <c r="G84" s="3"/>
-      <c r="H84" s="3"/>
-      <c r="I84" s="3"/>
-      <c r="J84" s="3"/>
-      <c r="K84" s="10"/>
-      <c r="L84" s="3"/>
-      <c r="M84" s="3"/>
-      <c r="N84" s="3"/>
-      <c r="O84" s="3"/>
+      <c r="A84" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D84" s="4">
+        <v>43322</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I84" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J84" s="3">
+        <v>2</v>
+      </c>
+      <c r="K84" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="L84" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M84" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N84" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O84" s="3" t="s">
+        <v>207</v>
+      </c>
       <c r="P84" s="3"/>
       <c r="Q84" s="3"/>
     </row>
@@ -5002,7 +5258,7 @@
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
       <c r="J85" s="3"/>
-      <c r="K85" s="3"/>
+      <c r="K85" s="10"/>
       <c r="L85" s="3"/>
       <c r="M85" s="3"/>
       <c r="N85" s="3"/>
@@ -5083,8 +5339,142 @@
       <c r="M89" s="3"/>
       <c r="N89" s="3"/>
       <c r="O89" s="3"/>
+      <c r="P89" s="3"/>
+      <c r="Q89" s="3"/>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A90" s="3"/>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="3"/>
+      <c r="I90" s="3"/>
+      <c r="J90" s="3"/>
+      <c r="K90" s="10"/>
+      <c r="L90" s="3"/>
+      <c r="M90" s="3"/>
+      <c r="N90" s="3"/>
+      <c r="O90" s="3"/>
+      <c r="P90" s="3"/>
+      <c r="Q90" s="3"/>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A91" s="3"/>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="4"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
+      <c r="I91" s="3"/>
+      <c r="J91" s="3"/>
+      <c r="K91" s="10"/>
+      <c r="L91" s="3"/>
+      <c r="M91" s="3"/>
+      <c r="N91" s="3"/>
+      <c r="O91" s="3"/>
+      <c r="P91" s="3"/>
+      <c r="Q91" s="3"/>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A92" s="3"/>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="4"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="4"/>
+      <c r="G92" s="3"/>
+      <c r="H92" s="3"/>
+      <c r="I92" s="3"/>
+      <c r="J92" s="3"/>
+      <c r="K92" s="3"/>
+      <c r="L92" s="3"/>
+      <c r="M92" s="3"/>
+      <c r="N92" s="3"/>
+      <c r="O92" s="3"/>
+      <c r="P92" s="3"/>
+      <c r="Q92" s="3"/>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A93" s="3"/>
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="3"/>
+      <c r="H93" s="3"/>
+      <c r="I93" s="3"/>
+      <c r="J93" s="3"/>
+      <c r="K93" s="10"/>
+      <c r="L93" s="3"/>
+      <c r="M93" s="3"/>
+      <c r="N93" s="3"/>
+      <c r="O93" s="3"/>
+      <c r="P93" s="3"/>
+      <c r="Q93" s="3"/>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A94" s="3"/>
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="4"/>
+      <c r="G94" s="3"/>
+      <c r="H94" s="3"/>
+      <c r="I94" s="3"/>
+      <c r="J94" s="3"/>
+      <c r="K94" s="10"/>
+      <c r="L94" s="3"/>
+      <c r="M94" s="3"/>
+      <c r="N94" s="3"/>
+      <c r="O94" s="3"/>
+      <c r="P94" s="3"/>
+      <c r="Q94" s="3"/>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A95" s="3"/>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4"/>
+      <c r="G95" s="3"/>
+      <c r="H95" s="3"/>
+      <c r="I95" s="3"/>
+      <c r="J95" s="3"/>
+      <c r="K95" s="10"/>
+      <c r="L95" s="3"/>
+      <c r="M95" s="3"/>
+      <c r="N95" s="3"/>
+      <c r="O95" s="3"/>
+      <c r="P95" s="3"/>
+      <c r="Q95" s="3"/>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A96" s="3"/>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="4"/>
+      <c r="G96" s="3"/>
+      <c r="H96" s="3"/>
+      <c r="I96" s="3"/>
+      <c r="J96" s="3"/>
+      <c r="K96" s="10"/>
+      <c r="L96" s="3"/>
+      <c r="M96" s="3"/>
+      <c r="N96" s="3"/>
+      <c r="O96" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated subject log 8/24, reached 50 kids
</commit_message>
<xml_diff>
--- a/data/01_participant_logs/es_combined_subject_log.xlsx
+++ b/data/01_participant_logs/es_combined_subject_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethswanson/Documents/speed-acc-novel/data/01_participant_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45403BF3-20C1-3343-A224-0A05C30122B2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83ECD3D6-3CA0-4D40-ADF6-8288AC6B96AC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25480" windowHeight="14760" xr2:uid="{C7933D04-C61A-4F49-A5A3-D50AD8D5C7BA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="259">
   <si>
     <t>subid</t>
   </si>
@@ -793,6 +793,15 @@
   </si>
   <si>
     <t>FS</t>
+  </si>
+  <si>
+    <t>SAN-082418-02</t>
+  </si>
+  <si>
+    <t>JMR</t>
+  </si>
+  <si>
+    <t>Mother sat in background; didn't distract him</t>
   </si>
 </sst>
 </file>
@@ -1199,10 +1208,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3EC3C8B-E78F-3A47-8874-F07602A94D1E}">
-  <dimension ref="A1:Q96"/>
+  <dimension ref="A1:Q97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4341,60 +4350,61 @@
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>158</v>
+        <v>256</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>159</v>
+        <v>257</v>
       </c>
       <c r="D66" s="4">
-        <v>43301</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>21</v>
+        <v>43336</v>
+      </c>
+      <c r="E66" s="4">
+        <v>41980</v>
+      </c>
+      <c r="F66" s="3">
+        <v>3.714</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>81</v>
+        <v>220</v>
       </c>
       <c r="I66" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J66" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K66" s="10" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="L66" s="3" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="M66" s="3" t="s">
-        <v>160</v>
+        <v>21</v>
       </c>
       <c r="N66" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O66" s="3" t="s">
-        <v>161</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="P66" s="3"/>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D67" s="4">
         <v>43301</v>
@@ -4415,33 +4425,33 @@
         <v>17</v>
       </c>
       <c r="J67" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K67" s="10" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="L67" s="3" t="s">
         <v>19</v>
       </c>
       <c r="M67" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="N67" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O67" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D68" s="4">
         <v>43301</v>
@@ -4453,7 +4463,7 @@
         <v>21</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H68" s="3" t="s">
         <v>81</v>
@@ -4462,10 +4472,10 @@
         <v>17</v>
       </c>
       <c r="J68" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K68" s="10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="L68" s="3" t="s">
         <v>19</v>
@@ -4477,21 +4487,21 @@
         <v>21</v>
       </c>
       <c r="O68" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D69" s="4">
-        <v>43306</v>
+        <v>43301</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>21</v>
@@ -4500,7 +4510,7 @@
         <v>21</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="H69" s="3" t="s">
         <v>81</v>
@@ -4509,33 +4519,33 @@
         <v>17</v>
       </c>
       <c r="J69" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K69" s="10" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="L69" s="3" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="M69" s="3" t="s">
-        <v>21</v>
+        <v>164</v>
       </c>
       <c r="N69" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O69" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D70" s="4">
         <v>43306</v>
@@ -4547,42 +4557,42 @@
         <v>21</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="I70" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J70" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K70" s="10" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="L70" s="3" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="M70" s="3" t="s">
-        <v>174</v>
+        <v>21</v>
       </c>
       <c r="N70" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O70" s="3" t="s">
-        <v>21</v>
+        <v>171</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D71" s="4">
         <v>43306</v>
@@ -4594,19 +4604,19 @@
         <v>21</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>81</v>
+        <v>26</v>
       </c>
       <c r="I71" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J71" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K71" s="10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="L71" s="3" t="s">
         <v>19</v>
@@ -4623,13 +4633,13 @@
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D72" s="4">
         <v>43306</v>
@@ -4650,10 +4660,10 @@
         <v>17</v>
       </c>
       <c r="J72" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K72" s="10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="L72" s="3" t="s">
         <v>19</v>
@@ -4670,16 +4680,16 @@
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D73" s="4">
-        <v>43308</v>
+        <v>43306</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>21</v>
@@ -4697,33 +4707,33 @@
         <v>17</v>
       </c>
       <c r="J73" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K73" s="10" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="L73" s="3" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="M73" s="3" t="s">
-        <v>21</v>
+        <v>174</v>
       </c>
       <c r="N73" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O73" s="3" t="s">
-        <v>181</v>
+        <v>21</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D74" s="4">
         <v>43308</v>
@@ -4744,33 +4754,33 @@
         <v>17</v>
       </c>
       <c r="J74" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K74" s="10" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="L74" s="3" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="M74" s="3" t="s">
-        <v>174</v>
+        <v>21</v>
       </c>
       <c r="N74" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O74" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>84</v>
+        <v>183</v>
       </c>
       <c r="D75" s="4">
         <v>43308</v>
@@ -4782,7 +4792,7 @@
         <v>21</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H75" s="3" t="s">
         <v>81</v>
@@ -4791,10 +4801,10 @@
         <v>17</v>
       </c>
       <c r="J75" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K75" s="10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="L75" s="3" t="s">
         <v>19</v>
@@ -4806,21 +4816,21 @@
         <v>21</v>
       </c>
       <c r="O75" s="3" t="s">
-        <v>21</v>
+        <v>184</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>187</v>
+        <v>84</v>
       </c>
       <c r="D76" s="4">
-        <v>43313</v>
+        <v>43308</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>21</v>
@@ -4829,25 +4839,25 @@
         <v>21</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="I76" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J76" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K76" s="10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="L76" s="3" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="M76" s="3" t="s">
-        <v>21</v>
+        <v>174</v>
       </c>
       <c r="N76" s="3" t="s">
         <v>21</v>
@@ -4858,13 +4868,13 @@
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D77" s="4">
         <v>43313</v>
@@ -4879,16 +4889,16 @@
         <v>15</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>190</v>
+        <v>77</v>
       </c>
       <c r="I77" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J77" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K77" s="10" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="L77" s="3" t="s">
         <v>40</v>
@@ -4902,17 +4912,16 @@
       <c r="O77" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="P77" s="3"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D78" s="4">
         <v>43313</v>
@@ -4924,19 +4933,19 @@
         <v>21</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>77</v>
+        <v>190</v>
       </c>
       <c r="I78" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J78" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K78" s="10" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="L78" s="3" t="s">
         <v>40</v>
@@ -4948,20 +4957,19 @@
         <v>21</v>
       </c>
       <c r="O78" s="3" t="s">
-        <v>193</v>
+        <v>21</v>
       </c>
       <c r="P78" s="3"/>
-      <c r="Q78" s="3"/>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D79" s="4">
         <v>43313</v>
@@ -4976,44 +4984,44 @@
         <v>25</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I79" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J79" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K79" s="10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="L79" s="3" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="M79" s="3" t="s">
-        <v>174</v>
+        <v>21</v>
       </c>
       <c r="N79" s="3" t="s">
         <v>21</v>
       </c>
       <c r="O79" s="3" t="s">
-        <v>21</v>
+        <v>193</v>
       </c>
       <c r="P79" s="3"/>
       <c r="Q79" s="3"/>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>117</v>
+        <v>195</v>
       </c>
       <c r="D80" s="4">
-        <v>43315</v>
+        <v>43313</v>
       </c>
       <c r="E80" s="4" t="s">
         <v>21</v>
@@ -5031,16 +5039,16 @@
         <v>17</v>
       </c>
       <c r="J80" s="3">
-        <v>4</v>
-      </c>
-      <c r="K80" s="3" t="s">
-        <v>50</v>
+        <v>3</v>
+      </c>
+      <c r="K80" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="L80" s="3" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="M80" s="3" t="s">
-        <v>21</v>
+        <v>174</v>
       </c>
       <c r="N80" s="3" t="s">
         <v>21</v>
@@ -5053,13 +5061,13 @@
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>198</v>
+        <v>117</v>
       </c>
       <c r="D81" s="4">
         <v>43315</v>
@@ -5071,19 +5079,19 @@
         <v>21</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="I81" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J81" s="3">
-        <v>3</v>
-      </c>
-      <c r="K81" s="10" t="s">
-        <v>45</v>
+        <v>4</v>
+      </c>
+      <c r="K81" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="L81" s="3" t="s">
         <v>40</v>
@@ -5102,16 +5110,16 @@
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D82" s="4">
-        <v>43318</v>
+        <v>43315</v>
       </c>
       <c r="E82" s="4" t="s">
         <v>21</v>
@@ -5120,7 +5128,7 @@
         <v>21</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H82" s="3" t="s">
         <v>77</v>
@@ -5129,10 +5137,10 @@
         <v>17</v>
       </c>
       <c r="J82" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K82" s="10" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="L82" s="3" t="s">
         <v>40</v>
@@ -5144,23 +5152,23 @@
         <v>21</v>
       </c>
       <c r="O82" s="3" t="s">
-        <v>201</v>
+        <v>21</v>
       </c>
       <c r="P82" s="3"/>
       <c r="Q82" s="3"/>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D83" s="4">
-        <v>43320</v>
+        <v>43318</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>21</v>
@@ -5178,10 +5186,10 @@
         <v>17</v>
       </c>
       <c r="J83" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K83" s="10" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="L83" s="3" t="s">
         <v>40</v>
@@ -5193,23 +5201,23 @@
         <v>21</v>
       </c>
       <c r="O83" s="3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="P83" s="3"/>
       <c r="Q83" s="3"/>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>211</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D84" s="4">
-        <v>43322</v>
+        <v>43320</v>
       </c>
       <c r="E84" s="4" t="s">
         <v>21</v>
@@ -5221,16 +5229,16 @@
         <v>25</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I84" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J84" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K84" s="10" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="L84" s="3" t="s">
         <v>40</v>
@@ -5242,27 +5250,57 @@
         <v>21</v>
       </c>
       <c r="O84" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="P84" s="3"/>
       <c r="Q84" s="3"/>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A85" s="3"/>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="4"/>
-      <c r="E85" s="4"/>
-      <c r="F85" s="4"/>
-      <c r="G85" s="3"/>
-      <c r="H85" s="3"/>
-      <c r="I85" s="3"/>
-      <c r="J85" s="3"/>
-      <c r="K85" s="10"/>
-      <c r="L85" s="3"/>
-      <c r="M85" s="3"/>
-      <c r="N85" s="3"/>
-      <c r="O85" s="3"/>
+      <c r="A85" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D85" s="4">
+        <v>43322</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H85" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I85" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J85" s="3">
+        <v>2</v>
+      </c>
+      <c r="K85" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="L85" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M85" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N85" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O85" s="3" t="s">
+        <v>207</v>
+      </c>
       <c r="P85" s="3"/>
       <c r="Q85" s="3"/>
     </row>
@@ -5391,7 +5429,7 @@
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
       <c r="J92" s="3"/>
-      <c r="K92" s="3"/>
+      <c r="K92" s="10"/>
       <c r="L92" s="3"/>
       <c r="M92" s="3"/>
       <c r="N92" s="3"/>
@@ -5410,7 +5448,7 @@
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
       <c r="J93" s="3"/>
-      <c r="K93" s="10"/>
+      <c r="K93" s="3"/>
       <c r="L93" s="3"/>
       <c r="M93" s="3"/>
       <c r="N93" s="3"/>
@@ -5472,6 +5510,25 @@
       <c r="M96" s="3"/>
       <c r="N96" s="3"/>
       <c r="O96" s="3"/>
+      <c r="P96" s="3"/>
+      <c r="Q96" s="3"/>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A97" s="3"/>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="3"/>
+      <c r="H97" s="3"/>
+      <c r="I97" s="3"/>
+      <c r="J97" s="3"/>
+      <c r="K97" s="10"/>
+      <c r="L97" s="3"/>
+      <c r="M97" s="3"/>
+      <c r="N97" s="3"/>
+      <c r="O97" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated adult data 10/18
</commit_message>
<xml_diff>
--- a/data/01_participant_logs/es_combined_subject_log.xlsx
+++ b/data/01_participant_logs/es_combined_subject_log.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethswanson/Documents/speed-acc-novel/data/01_participant_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83ECD3D6-3CA0-4D40-ADF6-8288AC6B96AC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C6793B-6189-B549-8404-80571139C33A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25480" windowHeight="14760" xr2:uid="{C7933D04-C61A-4F49-A5A3-D50AD8D5C7BA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25480" windowHeight="14540" xr2:uid="{C7933D04-C61A-4F49-A5A3-D50AD8D5C7BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179021"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="299">
   <si>
     <t>subid</t>
   </si>
@@ -802,6 +803,126 @@
   </si>
   <si>
     <t>Mother sat in background; didn't distract him</t>
+  </si>
+  <si>
+    <t>SAN-092718-01</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>SAN-092718-02</t>
+  </si>
+  <si>
+    <t>SAN-092718-03</t>
+  </si>
+  <si>
+    <t>SAN-092718-04</t>
+  </si>
+  <si>
+    <t>SAN-092718-05</t>
+  </si>
+  <si>
+    <t>CB</t>
+  </si>
+  <si>
+    <t>MH</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>SAN-092818-01</t>
+  </si>
+  <si>
+    <t>SJ</t>
+  </si>
+  <si>
+    <t>SAN-100418-01</t>
+  </si>
+  <si>
+    <t>SAN-100418-02</t>
+  </si>
+  <si>
+    <t>SAN-100418-03</t>
+  </si>
+  <si>
+    <t>SAN-100418-04</t>
+  </si>
+  <si>
+    <t>SAN-100418-05</t>
+  </si>
+  <si>
+    <t>TW</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>JH</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C, A </t>
+  </si>
+  <si>
+    <t>Seemed quite intent on looking at right answer</t>
+  </si>
+  <si>
+    <t>SAN-100518-01</t>
+  </si>
+  <si>
+    <t>SAN-100518-02</t>
+  </si>
+  <si>
+    <t>SAN-100518-03</t>
+  </si>
+  <si>
+    <t>SAN-100518-04</t>
+  </si>
+  <si>
+    <t>JT</t>
+  </si>
+  <si>
+    <t>MR</t>
+  </si>
+  <si>
+    <t>EB</t>
+  </si>
+  <si>
+    <t>C, H, A</t>
+  </si>
+  <si>
+    <t>A, H?</t>
+  </si>
+  <si>
+    <t>SAN-100818-01</t>
+  </si>
+  <si>
+    <t>SAN-100918-01</t>
+  </si>
+  <si>
+    <t>NB</t>
+  </si>
+  <si>
+    <t>SAN-101718-01</t>
+  </si>
+  <si>
+    <t>SAN-101818-01</t>
+  </si>
+  <si>
+    <t>MY</t>
+  </si>
+  <si>
+    <t>C, A</t>
+  </si>
+  <si>
+    <t>SAN-101818-02</t>
+  </si>
+  <si>
+    <t>MG</t>
   </si>
 </sst>
 </file>
@@ -880,7 +1001,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -894,6 +1015,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1208,10 +1330,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3EC3C8B-E78F-3A47-8874-F07602A94D1E}">
-  <dimension ref="A1:Q97"/>
+  <dimension ref="A1:Q106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="O106" sqref="O106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5305,230 +5427,972 @@
       <c r="Q85" s="3"/>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A86" s="3"/>
-      <c r="B86" s="3"/>
-      <c r="C86" s="3"/>
-      <c r="D86" s="4"/>
-      <c r="E86" s="4"/>
-      <c r="F86" s="4"/>
-      <c r="G86" s="3"/>
-      <c r="H86" s="3"/>
-      <c r="I86" s="3"/>
-      <c r="J86" s="3"/>
-      <c r="K86" s="10"/>
-      <c r="L86" s="3"/>
-      <c r="M86" s="3"/>
-      <c r="N86" s="3"/>
-      <c r="O86" s="3"/>
+      <c r="A86" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="D86" s="4">
+        <v>43370</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I86" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J86" s="3">
+        <v>3</v>
+      </c>
+      <c r="K86" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="L86" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M86" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N86" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O86" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="P86" s="3"/>
       <c r="Q86" s="3"/>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A87" s="3"/>
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="4"/>
-      <c r="E87" s="4"/>
-      <c r="F87" s="4"/>
-      <c r="G87" s="3"/>
-      <c r="H87" s="3"/>
-      <c r="I87" s="3"/>
-      <c r="J87" s="3"/>
-      <c r="K87" s="10"/>
-      <c r="L87" s="3"/>
-      <c r="M87" s="3"/>
-      <c r="N87" s="3"/>
-      <c r="O87" s="3"/>
+      <c r="A87" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D87" s="4">
+        <v>43370</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H87" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I87" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J87" s="3">
+        <v>3</v>
+      </c>
+      <c r="K87" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="L87" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M87" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N87" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O87" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="P87" s="3"/>
       <c r="Q87" s="3"/>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A88" s="3"/>
-      <c r="B88" s="3"/>
-      <c r="C88" s="3"/>
-      <c r="D88" s="4"/>
-      <c r="E88" s="4"/>
-      <c r="F88" s="4"/>
-      <c r="G88" s="3"/>
-      <c r="H88" s="3"/>
-      <c r="I88" s="3"/>
-      <c r="J88" s="3"/>
-      <c r="K88" s="10"/>
-      <c r="L88" s="3"/>
-      <c r="M88" s="3"/>
-      <c r="N88" s="3"/>
-      <c r="O88" s="3"/>
+      <c r="A88" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D88" s="4">
+        <v>43370</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I88" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J88" s="3">
+        <v>3</v>
+      </c>
+      <c r="K88" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="L88" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M88" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N88" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O88" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="P88" s="3"/>
       <c r="Q88" s="3"/>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A89" s="3"/>
-      <c r="B89" s="3"/>
-      <c r="C89" s="3"/>
-      <c r="D89" s="4"/>
-      <c r="E89" s="4"/>
-      <c r="F89" s="4"/>
-      <c r="G89" s="3"/>
-      <c r="H89" s="3"/>
-      <c r="I89" s="3"/>
-      <c r="J89" s="3"/>
-      <c r="K89" s="10"/>
-      <c r="L89" s="3"/>
-      <c r="M89" s="3"/>
-      <c r="N89" s="3"/>
-      <c r="O89" s="3"/>
+      <c r="A89" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D89" s="4">
+        <v>43370</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I89" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J89" s="3">
+        <v>4</v>
+      </c>
+      <c r="K89" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L89" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M89" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N89" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O89" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="P89" s="3"/>
       <c r="Q89" s="3"/>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A90" s="3"/>
-      <c r="B90" s="3"/>
-      <c r="C90" s="3"/>
-      <c r="D90" s="4"/>
-      <c r="E90" s="4"/>
-      <c r="F90" s="4"/>
-      <c r="G90" s="3"/>
-      <c r="H90" s="3"/>
-      <c r="I90" s="3"/>
-      <c r="J90" s="3"/>
-      <c r="K90" s="10"/>
-      <c r="L90" s="3"/>
-      <c r="M90" s="3"/>
-      <c r="N90" s="3"/>
-      <c r="O90" s="3"/>
+      <c r="A90" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D90" s="4">
+        <v>43370</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I90" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J90" s="3">
+        <v>4</v>
+      </c>
+      <c r="K90" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L90" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M90" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N90" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O90" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="P90" s="3"/>
       <c r="Q90" s="3"/>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A91" s="3"/>
-      <c r="B91" s="3"/>
-      <c r="C91" s="3"/>
-      <c r="D91" s="4"/>
-      <c r="E91" s="4"/>
-      <c r="F91" s="4"/>
-      <c r="G91" s="3"/>
-      <c r="H91" s="3"/>
-      <c r="I91" s="3"/>
-      <c r="J91" s="3"/>
-      <c r="K91" s="10"/>
-      <c r="L91" s="3"/>
-      <c r="M91" s="3"/>
-      <c r="N91" s="3"/>
-      <c r="O91" s="3"/>
+      <c r="A91" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="D91" s="4">
+        <v>43371</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I91" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J91" s="3">
+        <v>2</v>
+      </c>
+      <c r="K91" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="L91" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M91" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N91" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O91" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="P91" s="3"/>
       <c r="Q91" s="3"/>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A92" s="3"/>
-      <c r="B92" s="3"/>
-      <c r="C92" s="3"/>
-      <c r="D92" s="4"/>
-      <c r="E92" s="4"/>
-      <c r="F92" s="4"/>
-      <c r="G92" s="3"/>
-      <c r="H92" s="3"/>
-      <c r="I92" s="3"/>
-      <c r="J92" s="3"/>
-      <c r="K92" s="10"/>
-      <c r="L92" s="3"/>
-      <c r="M92" s="3"/>
-      <c r="N92" s="3"/>
-      <c r="O92" s="3"/>
+      <c r="A92" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D92" s="4">
+        <v>43377</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I92" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J92" s="3">
+        <v>1</v>
+      </c>
+      <c r="K92" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L92" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M92" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N92" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O92" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="P92" s="3"/>
       <c r="Q92" s="3"/>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A93" s="3"/>
-      <c r="B93" s="3"/>
-      <c r="C93" s="3"/>
-      <c r="D93" s="4"/>
-      <c r="E93" s="4"/>
-      <c r="F93" s="4"/>
-      <c r="G93" s="3"/>
-      <c r="H93" s="3"/>
-      <c r="I93" s="3"/>
-      <c r="J93" s="3"/>
-      <c r="K93" s="3"/>
-      <c r="L93" s="3"/>
-      <c r="M93" s="3"/>
-      <c r="N93" s="3"/>
-      <c r="O93" s="3"/>
+      <c r="A93" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="D93" s="4">
+        <v>43377</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H93" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="I93" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J93" s="3">
+        <v>2</v>
+      </c>
+      <c r="K93" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="L93" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M93" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N93" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O93" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="P93" s="3"/>
       <c r="Q93" s="3"/>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A94" s="3"/>
-      <c r="B94" s="3"/>
-      <c r="C94" s="3"/>
-      <c r="D94" s="4"/>
-      <c r="E94" s="4"/>
-      <c r="F94" s="4"/>
-      <c r="G94" s="3"/>
-      <c r="H94" s="3"/>
-      <c r="I94" s="3"/>
-      <c r="J94" s="3"/>
-      <c r="K94" s="10"/>
-      <c r="L94" s="3"/>
-      <c r="M94" s="3"/>
-      <c r="N94" s="3"/>
-      <c r="O94" s="3"/>
+      <c r="A94" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D94" s="4">
+        <v>43377</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I94" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J94" s="3">
+        <v>2</v>
+      </c>
+      <c r="K94" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="L94" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M94" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N94" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O94" s="3" t="s">
+        <v>280</v>
+      </c>
       <c r="P94" s="3"/>
       <c r="Q94" s="3"/>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A95" s="3"/>
-      <c r="B95" s="3"/>
-      <c r="C95" s="3"/>
-      <c r="D95" s="4"/>
-      <c r="E95" s="4"/>
-      <c r="F95" s="4"/>
-      <c r="G95" s="3"/>
-      <c r="H95" s="3"/>
-      <c r="I95" s="3"/>
-      <c r="J95" s="3"/>
-      <c r="K95" s="10"/>
-      <c r="L95" s="3"/>
-      <c r="M95" s="3"/>
-      <c r="N95" s="3"/>
-      <c r="O95" s="3"/>
+      <c r="A95" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="D95" s="4">
+        <v>43377</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H95" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I95" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J95" s="3">
+        <v>3</v>
+      </c>
+      <c r="K95" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="L95" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M95" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N95" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O95" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="P95" s="3"/>
       <c r="Q95" s="3"/>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A96" s="3"/>
-      <c r="B96" s="3"/>
-      <c r="C96" s="3"/>
-      <c r="D96" s="4"/>
-      <c r="E96" s="4"/>
-      <c r="F96" s="4"/>
-      <c r="G96" s="3"/>
-      <c r="H96" s="3"/>
-      <c r="I96" s="3"/>
-      <c r="J96" s="3"/>
-      <c r="K96" s="10"/>
-      <c r="L96" s="3"/>
-      <c r="M96" s="3"/>
-      <c r="N96" s="3"/>
-      <c r="O96" s="3"/>
+      <c r="A96" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D96" s="4">
+        <v>43377</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I96" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J96" s="3">
+        <v>4</v>
+      </c>
+      <c r="K96" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L96" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M96" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N96" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O96" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="P96" s="3"/>
       <c r="Q96" s="3"/>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A97" s="3"/>
-      <c r="B97" s="3"/>
-      <c r="C97" s="3"/>
-      <c r="D97" s="4"/>
-      <c r="E97" s="4"/>
-      <c r="F97" s="4"/>
-      <c r="G97" s="3"/>
-      <c r="H97" s="3"/>
-      <c r="I97" s="3"/>
-      <c r="J97" s="3"/>
-      <c r="K97" s="10"/>
-      <c r="L97" s="3"/>
-      <c r="M97" s="3"/>
-      <c r="N97" s="3"/>
-      <c r="O97" s="3"/>
+      <c r="A97" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D97" s="4">
+        <v>43378</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H97" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="I97" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J97" s="3">
+        <v>1</v>
+      </c>
+      <c r="K97" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L97" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M97" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N97" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O97" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="D98" s="4">
+        <v>43378</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H98" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I98" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J98" s="3">
+        <v>2</v>
+      </c>
+      <c r="K98" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="L98" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M98" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N98" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O98" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A99" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D99" s="4">
+        <v>43378</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H99" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="I99" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J99" s="3">
+        <v>2</v>
+      </c>
+      <c r="K99" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="L99" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M99" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N99" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O99" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A100" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="D100" s="4">
+        <v>43378</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H100" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I100" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J100" s="3">
+        <v>3</v>
+      </c>
+      <c r="K100" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="L100" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M100" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N100" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O100" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="D101" s="11">
+        <v>43381</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H101" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I101" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J101" s="3">
+        <v>4</v>
+      </c>
+      <c r="K101" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L101" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M101" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N101" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O101" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="D102" s="11">
+        <v>43382</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H102" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I102" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J102" s="3">
+        <v>4</v>
+      </c>
+      <c r="K102" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L102" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M102" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N102" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O102" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A103" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="D103" s="11">
+        <v>43390</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H103" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="I103" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J103" s="3">
+        <v>4</v>
+      </c>
+      <c r="K103" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L103" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M103" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N103" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O103" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D104" s="11">
+        <v>43391</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H104" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J104" s="3">
+        <v>4</v>
+      </c>
+      <c r="K104" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L104" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M104" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N104" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O104" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A105" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D105" s="11">
+        <v>43391</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F105" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G105" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H105" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I105" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J105" s="3">
+        <v>3</v>
+      </c>
+      <c r="K105" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="L105" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M105" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N105" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O105" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B106" s="3"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4"/>
+      <c r="I106" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>